<commit_message>
change Campaign to Topic
</commit_message>
<xml_diff>
--- a/data/dummy/advocacy_impact_dummy_data.xlsx
+++ b/data/dummy/advocacy_impact_dummy_data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmatton/climact_dev/hackaton_ecf_aim/data/dummy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9828ECB-7FFD-9F41-BC73-77410D22B187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E9BC34-C0FE-3D47-BD1B-C8EDE8E5FD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentions_support" sheetId="1" r:id="rId1"/>
-    <sheet name="campaign_mentions" sheetId="2" r:id="rId2"/>
+    <sheet name="topic_mentions" sheetId="2" r:id="rId2"/>
     <sheet name="mep_sentiment" sheetId="3" r:id="rId3"/>
-    <sheet name="campaigns" sheetId="4" r:id="rId4"/>
+    <sheet name="interventions" sheetId="4" r:id="rId4"/>
     <sheet name="voting_results" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -35,9 +35,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>sentiment</t>
   </si>
   <si>
@@ -65,7 +62,7 @@
     <t>DUMMY</t>
   </si>
   <si>
-    <t>Car taxation</t>
+    <t>topic</t>
   </si>
   <si>
     <t>Climate policy</t>
@@ -74,9 +71,6 @@
     <t>Green energy subsidies</t>
   </si>
   <si>
-    <t>campaign</t>
-  </si>
-  <si>
     <t>positive</t>
   </si>
   <si>
@@ -168,6 +162,12 @@
   </si>
   <si>
     <t>tweet</t>
+  </si>
+  <si>
+    <t>Nature Restauration Law</t>
+  </si>
+  <si>
+    <t>content</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -606,7 +606,7 @@
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -617,7 +617,7 @@
         <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +630,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -646,13 +646,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -660,13 +660,13 @@
         <v>45293</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -674,13 +674,13 @@
         <v>45325</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -688,13 +688,13 @@
         <v>45355</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -702,13 +702,13 @@
         <v>45387</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -716,13 +716,13 @@
         <v>45418</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -730,13 +730,13 @@
         <v>45449</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -744,13 +744,13 @@
         <v>45480</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,13 +758,13 @@
         <v>45511</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -772,13 +772,13 @@
         <v>45542</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -786,13 +786,13 @@
         <v>45573</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -800,13 +800,13 @@
         <v>45293</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -814,13 +814,13 @@
         <v>45325</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -828,13 +828,13 @@
         <v>45355</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -842,13 +842,13 @@
         <v>45387</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -856,13 +856,13 @@
         <v>45418</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -870,13 +870,13 @@
         <v>45449</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -884,13 +884,13 @@
         <v>45480</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -898,13 +898,13 @@
         <v>45511</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -912,13 +912,13 @@
         <v>45542</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -926,13 +926,13 @@
         <v>45573</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -945,7 +945,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -962,19 +962,19 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -985,16 +985,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1005,16 +1005,16 @@
         <v>-1</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1025,16 +1025,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1045,16 +1045,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1065,16 +1065,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1085,16 +1085,16 @@
         <v>-1</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1105,16 +1105,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1125,16 +1125,16 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1145,16 +1145,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1165,16 +1165,16 @@
         <v>-1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1185,16 +1185,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1205,16 +1205,16 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1227,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1240,19 +1240,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1260,16 +1260,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3">
         <v>45293</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1277,16 +1277,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3">
         <v>45325</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1294,16 +1294,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3">
         <v>45355</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1311,16 +1311,16 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3">
         <v>45387</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1328,16 +1328,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3">
         <v>45418</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1345,16 +1345,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C7" s="3">
         <v>45449</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,16 +1362,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3">
         <v>45480</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1379,16 +1379,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3">
         <v>45511</v>
       </c>
       <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1396,16 +1396,16 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3">
         <v>45542</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1413,16 +1413,16 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3">
         <v>45573</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1470,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1484,16 +1484,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1507,7 +1507,7 @@
         <v>720</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1521,7 +1521,7 @@
         <v>720</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1535,12 +1535,12 @@
         <v>720</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>